<commit_message>
Feat: Implemented Applications used
- Invoked UiDemo_Open workflow in InitApplications
- Invoved UiDemo_ForceClose workflow in KillAllProcesses
- Invoked UiDemo_Close workflow in CloseAllApplications
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1622,8 +1622,6 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix: End to end testing changes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -162,10 +162,10 @@
     <t>Create a generic credential on Credential Manager on Windows. Credential Manager &gt; Windows Credential</t>
   </si>
   <si>
-    <t>ManualTransactonThreshold</t>
-  </si>
-  <si>
     <t>Data\Input\UiDemo-Transactions.xlsx</t>
+  </si>
+  <si>
+    <t>ManualTransactionThreshold</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -626,13 +626,13 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <v>10000</v>

</xml_diff>

<commit_message>
Feat: Implemented all Unit Test Cases
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1646,7 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>